<commit_message>
refactored base-delta with prints
</commit_message>
<xml_diff>
--- a/documents/data/cache-config.xlsx
+++ b/documents/data/cache-config.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
improved locality for bisort pool test
</commit_message>
<xml_diff>
--- a/documents/data/cache-config.xlsx
+++ b/documents/data/cache-config.xlsx
@@ -4,15 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="340" windowWidth="25360" windowHeight="17320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27120" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -169,10 +166,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -351,13 +348,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.567165427789565</c:v>
+                  <c:v>0.968642352183527</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.696665287349587</c:v>
+                  <c:v>1.004763221303491</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.929265421243451</c:v>
+                  <c:v>1.028594183648593</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.002501855976244</c:v>
@@ -490,13 +487,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.126968608303736</c:v>
+                  <c:v>1.151292819571437</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.089250664635531</c:v>
+                  <c:v>1.098320284749636</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.050589642796103</c:v>
+                  <c:v>1.054384386546792</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.002501855976244</c:v>
@@ -517,11 +514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2130274040"/>
-        <c:axId val="-2143193352"/>
+        <c:axId val="2078396760"/>
+        <c:axId val="2115926392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2130274040"/>
+        <c:axId val="2078396760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,7 +528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143193352"/>
+        <c:crossAx val="2115926392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -539,7 +536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143193352"/>
+        <c:axId val="2115926392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130274040"/>
+        <c:crossAx val="2078396760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -928,19 +925,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.023489074254132</c:v>
+                  <c:v>1.0307020369249</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.026565592729349</c:v>
+                  <c:v>1.024767345788526</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.016376364167651</c:v>
+                  <c:v>1.143655659576597</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.777038203794974</c:v>
+                  <c:v>2.25146141314941</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.806592935092503</c:v>
+                  <c:v>2.287311319153194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -955,11 +952,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2139285048"/>
-        <c:axId val="-2144359032"/>
+        <c:axId val="2115818360"/>
+        <c:axId val="2115837016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2139285048"/>
+        <c:axId val="2115818360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +966,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144359032"/>
+        <c:crossAx val="2115837016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -977,7 +974,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144359032"/>
+        <c:axId val="2115837016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1022,7 +1019,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139285048"/>
+        <c:crossAx val="2115818360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1405,11 +1402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2125771304"/>
-        <c:axId val="-2130461592"/>
+        <c:axId val="2121858440"/>
+        <c:axId val="2121861496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2125771304"/>
+        <c:axId val="2121858440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1419,7 +1416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130461592"/>
+        <c:crossAx val="2121861496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1427,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130461592"/>
+        <c:axId val="2121861496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,7 +1469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125771304"/>
+        <c:crossAx val="2121858440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1855,11 +1852,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124907832"/>
-        <c:axId val="-2125261320"/>
+        <c:axId val="2115938696"/>
+        <c:axId val="2115941752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124907832"/>
+        <c:axId val="2115938696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1869,7 +1866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125261320"/>
+        <c:crossAx val="2115941752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1877,7 +1874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125261320"/>
+        <c:axId val="2115941752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1922,7 +1919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124907832"/>
+        <c:crossAx val="2115938696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2281,11 +2278,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2128309592"/>
-        <c:axId val="2133959640"/>
+        <c:axId val="2115844840"/>
+        <c:axId val="2115847896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128309592"/>
+        <c:axId val="2115844840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,7 +2292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133959640"/>
+        <c:crossAx val="2115847896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2303,7 +2300,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133959640"/>
+        <c:axId val="2115847896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2348,7 +2345,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128309592"/>
+        <c:crossAx val="2115844840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2707,11 +2704,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2120453000"/>
-        <c:axId val="-2124070520"/>
+        <c:axId val="2123561176"/>
+        <c:axId val="2123564232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2120453000"/>
+        <c:axId val="2123561176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2721,7 +2718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124070520"/>
+        <c:crossAx val="2123564232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2729,7 +2726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124070520"/>
+        <c:axId val="2123564232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2774,7 +2771,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120453000"/>
+        <c:crossAx val="2123561176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3015,73 +3012,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>bisort</v>
-          </cell>
-          <cell r="F30">
-            <v>1</v>
-          </cell>
-          <cell r="G30">
-            <v>0.625</v>
-          </cell>
-          <cell r="H30">
-            <v>0.87353437499999997</v>
-          </cell>
-          <cell r="I30">
-            <v>0.55078125</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>llu</v>
-          </cell>
-          <cell r="F31">
-            <v>1</v>
-          </cell>
-          <cell r="G31">
-            <v>0.75340028384456359</v>
-          </cell>
-          <cell r="H31">
-            <v>0.9828883134652141</v>
-          </cell>
-          <cell r="I31">
-            <v>0.26828412060693529</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>sort</v>
-          </cell>
-          <cell r="F32">
-            <v>1</v>
-          </cell>
-          <cell r="G32">
-            <v>0.81673306772908372</v>
-          </cell>
-          <cell r="H32">
-            <v>0.952191235059761</v>
-          </cell>
-          <cell r="I32">
-            <v>0.44223107569721115</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3408,8 +3338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3488,13 +3418,13 @@
         <v>1027947</v>
       </c>
       <c r="D6" s="4">
-        <v>583016</v>
+        <v>995713</v>
       </c>
       <c r="E6" s="4">
         <v>1160562</v>
       </c>
       <c r="F6" s="4">
-        <v>1158464</v>
+        <v>1183468</v>
       </c>
       <c r="G6" s="3">
         <f>C6/B6</f>
@@ -3502,7 +3432,7 @@
       </c>
       <c r="H6" s="3">
         <f>D6/B6</f>
-        <v>0.47870872071684456</v>
+        <v>0.81757018063163189</v>
       </c>
       <c r="I6" s="3">
         <f>E6/B6</f>
@@ -3510,7 +3440,7 @@
       </c>
       <c r="J6" s="3">
         <f>F6/B6</f>
-        <v>0.95120343084326786</v>
+        <v>0.97173397006140938</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -3524,13 +3454,13 @@
         <v>1092328</v>
       </c>
       <c r="D7" s="4">
-        <v>760987</v>
+        <v>1097531</v>
       </c>
       <c r="E7" s="4">
         <v>1175680</v>
       </c>
       <c r="F7" s="4">
-        <v>1189819</v>
+        <v>1199726</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" ref="G7:G11" si="0">C7/B7</f>
@@ -3538,7 +3468,7 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" ref="H7:H11" si="1">D7/B7</f>
-        <v>0.62483896368564396</v>
+        <v>0.90117194203431661</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" ref="I7:I11" si="2">E7/B7</f>
@@ -3546,7 +3476,7 @@
       </c>
       <c r="J7" s="3">
         <f t="shared" ref="J7:J11" si="3">F7/B7</f>
-        <v>0.97694871388537419</v>
+        <v>0.98508325444025047</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3560,13 +3490,13 @@
         <v>1152647</v>
       </c>
       <c r="D8" s="4">
-        <v>1071115</v>
+        <v>1185606</v>
       </c>
       <c r="E8" s="4">
         <v>1189731</v>
       </c>
       <c r="F8" s="4">
-        <v>1210959</v>
+        <v>1215333</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
@@ -3574,7 +3504,7 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>0.87948202346183124</v>
+        <v>0.9734894608968111</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="2"/>
@@ -3582,7 +3512,7 @@
       </c>
       <c r="J8" s="3">
         <f t="shared" si="3"/>
-        <v>0.99430656059276146</v>
+        <v>0.99789800910260584</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3694,117 +3624,117 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f>G6/G6</f>
         <v>1</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <f>H6/G6</f>
-        <v>0.56716542778956502</v>
-      </c>
-      <c r="I13" s="6">
+        <v>0.96864235218352701</v>
+      </c>
+      <c r="I13" s="5">
         <f>I6/G6</f>
         <v>1.1290095695595201</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <f>J6/G6</f>
-        <v>1.1269686083037356</v>
+        <v>1.1512928195714371</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <f t="shared" ref="G14:G18" si="4">G7/G7</f>
         <v>1</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <f t="shared" ref="H14:H18" si="5">H7/G7</f>
-        <v>0.69666528734958721</v>
-      </c>
-      <c r="I14" s="6">
+        <v>1.0047632213034912</v>
+      </c>
+      <c r="I14" s="5">
         <f t="shared" ref="I14:I18" si="6">I7/G7</f>
         <v>1.0763067503533736</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <f t="shared" ref="J14:J18" si="7">J7/G7</f>
-        <v>1.0892506646355307</v>
+        <v>1.0983202847496356</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f t="shared" si="5"/>
-        <v>0.92926542124345102</v>
-      </c>
-      <c r="I15" s="6">
+        <v>1.0285941836485932</v>
+      </c>
+      <c r="I15" s="5">
         <f t="shared" si="6"/>
         <v>1.0321729028922124</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <f t="shared" si="7"/>
-        <v>1.0505896427961032</v>
+        <v>1.0543843865467919</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="5"/>
         <v>1.0025018559762435</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <f t="shared" si="6"/>
         <v>1.0011869999175123</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <f t="shared" si="7"/>
         <v>1.0025018559762435</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <f t="shared" si="5"/>
         <v>1.0012654504830709</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <f t="shared" si="7"/>
         <v>1.0012654504830709</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <f t="shared" si="5"/>
         <v>1.0012654504830709</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <f t="shared" si="7"/>
         <v>1.0012654504830709</v>
       </c>
@@ -3866,23 +3796,23 @@
         <v>15.5078</v>
       </c>
       <c r="F22" s="4">
-        <v>15.6328</v>
+        <v>15.523400000000001</v>
       </c>
       <c r="G22" s="3">
-        <f>C22/A22</f>
+        <f t="shared" ref="G22:G27" si="8">C22/A22</f>
         <v>1</v>
       </c>
       <c r="H22" s="3">
-        <f>D22/A22</f>
+        <f t="shared" ref="H22:H27" si="9">D22/A22</f>
         <v>1</v>
       </c>
       <c r="I22" s="3">
-        <f>E22/A22</f>
+        <f t="shared" ref="I22:I27" si="10">E22/A22</f>
         <v>0.96923749999999997</v>
       </c>
       <c r="J22" s="3">
-        <f>F22/A22</f>
-        <v>0.97704999999999997</v>
+        <f t="shared" ref="J22:J27" si="11">F22/A22</f>
+        <v>0.97021250000000003</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -3899,23 +3829,23 @@
         <v>30.984400000000001</v>
       </c>
       <c r="F23" s="4">
-        <v>31.171900000000001</v>
+        <v>31.226600000000001</v>
       </c>
       <c r="G23" s="3">
-        <f>C23/A23</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H23" s="3">
-        <f>D23/A23</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I23" s="3">
-        <f>E23/A23</f>
+        <f t="shared" si="10"/>
         <v>0.96826250000000003</v>
       </c>
       <c r="J23" s="3">
-        <f>F23/A23</f>
-        <v>0.97412187500000003</v>
+        <f t="shared" si="11"/>
+        <v>0.97583125000000004</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -3932,23 +3862,23 @@
         <v>62.695300000000003</v>
       </c>
       <c r="F24" s="4">
-        <v>62.968800000000002</v>
+        <v>55.960900000000002</v>
       </c>
       <c r="G24" s="3">
-        <f>C24/A24</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="H24" s="3">
-        <f>D24/A24</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="I24" s="3">
-        <f>E24/A24</f>
+        <f t="shared" si="10"/>
         <v>0.97961406250000005</v>
       </c>
       <c r="J24" s="3">
-        <f>F24/A24</f>
-        <v>0.98388750000000003</v>
+        <f t="shared" si="11"/>
+        <v>0.87438906250000004</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -3965,23 +3895,23 @@
         <v>106.062</v>
       </c>
       <c r="F25" s="4">
-        <v>70.851600000000005</v>
+        <v>55.921900000000001</v>
       </c>
       <c r="G25" s="3">
-        <f>C25/A25</f>
+        <f t="shared" si="8"/>
         <v>0.98364062500000005</v>
       </c>
       <c r="H25" s="3">
-        <f>D25/A25</f>
+        <f t="shared" si="9"/>
         <v>0.625</v>
       </c>
       <c r="I25" s="3">
-        <f>E25/A25</f>
+        <f t="shared" si="10"/>
         <v>0.82860937499999998</v>
       </c>
       <c r="J25" s="3">
-        <f>F25/A25</f>
-        <v>0.55352812500000004</v>
+        <f t="shared" si="11"/>
+        <v>0.43688984375000001</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -3998,23 +3928,23 @@
         <v>106.117</v>
       </c>
       <c r="F26" s="4">
-        <v>70.851600000000005</v>
+        <v>55.960900000000002</v>
       </c>
       <c r="G26" s="3">
-        <f>C26/A26</f>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="H26" s="3">
-        <f>D26/A26</f>
+        <f t="shared" si="9"/>
         <v>0.3125</v>
       </c>
       <c r="I26" s="3">
-        <f>E26/A26</f>
+        <f t="shared" si="10"/>
         <v>0.41451953125000002</v>
       </c>
       <c r="J26" s="3">
-        <f>F26/A26</f>
-        <v>0.27676406250000002</v>
+        <f t="shared" si="11"/>
+        <v>0.21859726562500001</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -4024,30 +3954,26 @@
       <c r="C27" s="4">
         <v>128</v>
       </c>
-      <c r="D27" s="4">
-        <v>80</v>
-      </c>
+      <c r="D27" s="4"/>
       <c r="E27" s="4">
         <v>106.117</v>
       </c>
-      <c r="F27" s="4">
-        <v>70.851600000000005</v>
-      </c>
+      <c r="F27" s="4"/>
       <c r="G27" s="3">
-        <f>C27/A27</f>
+        <f t="shared" si="8"/>
         <v>0.25</v>
       </c>
       <c r="H27" s="3">
-        <f>D27/A27</f>
-        <v>0.15625</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="I27" s="3">
-        <f>E27/A27</f>
+        <f t="shared" si="10"/>
         <v>0.20725976562500001</v>
       </c>
       <c r="J27" s="3">
-        <f>F27/A27</f>
-        <v>0.13838203125000001</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -4056,118 +3982,118 @@
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <f>G22/G22</f>
         <v>1</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <f>G22/H22</f>
         <v>1</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="5">
         <f>G22/I22</f>
         <v>1.0317388668927894</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="5">
         <f>G22/J22</f>
-        <v>1.0234890742541323</v>
+        <v>1.0307020369249005</v>
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="G30" s="6">
-        <f t="shared" ref="G30:G34" si="8">G23/G23</f>
-        <v>1</v>
-      </c>
-      <c r="H30" s="6">
-        <f t="shared" ref="H30:H34" si="9">G23/H23</f>
-        <v>1</v>
-      </c>
-      <c r="I30" s="6">
-        <f t="shared" ref="I30:I34" si="10">G23/I23</f>
+      <c r="G30" s="5">
+        <f t="shared" ref="G30:G34" si="12">G23/G23</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" ref="H30:H34" si="13">G23/H23</f>
+        <v>1</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" ref="I30:I34" si="14">G23/I23</f>
         <v>1.0327777849498456</v>
       </c>
-      <c r="J30" s="6">
-        <f t="shared" ref="J30:J34" si="11">G23/J23</f>
-        <v>1.0265655927293491</v>
+      <c r="J30" s="5">
+        <f t="shared" ref="J30:J34" si="15">G23/J23</f>
+        <v>1.0247673457885265</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="G31" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H31" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="I31" s="6">
-        <f t="shared" si="10"/>
+      <c r="G31" s="5">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" si="14"/>
         <v>1.0208101723733676</v>
       </c>
-      <c r="J31" s="6">
-        <f t="shared" si="11"/>
-        <v>1.0163763641676513</v>
+      <c r="J31" s="5">
+        <f t="shared" si="15"/>
+        <v>1.1436556595765972</v>
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="G32" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H32" s="6">
-        <f t="shared" si="9"/>
+      <c r="G32" s="5">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" si="13"/>
         <v>1.573825</v>
       </c>
-      <c r="I32" s="6">
-        <f t="shared" si="10"/>
+      <c r="I32" s="5">
+        <f t="shared" si="14"/>
         <v>1.1870981124248081</v>
       </c>
-      <c r="J32" s="6">
-        <f t="shared" si="11"/>
-        <v>1.7770382037949743</v>
+      <c r="J32" s="5">
+        <f t="shared" si="15"/>
+        <v>2.2514614131494102</v>
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="G33" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H33" s="6">
-        <f t="shared" si="9"/>
+      <c r="G33" s="5">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="13"/>
         <v>1.6</v>
       </c>
-      <c r="I33" s="6">
-        <f t="shared" si="10"/>
+      <c r="I33" s="5">
+        <f t="shared" si="14"/>
         <v>1.2062157806948932</v>
       </c>
-      <c r="J33" s="6">
-        <f t="shared" si="11"/>
-        <v>1.8065929350925032</v>
+      <c r="J33" s="5">
+        <f t="shared" si="15"/>
+        <v>2.2873113191531944</v>
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="G34" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H34" s="6">
-        <f t="shared" si="9"/>
-        <v>1.6</v>
-      </c>
-      <c r="I34" s="6">
-        <f t="shared" si="10"/>
+      <c r="G34" s="5">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="H34" s="5" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="5">
+        <f t="shared" si="14"/>
         <v>1.2062157806948932</v>
       </c>
-      <c r="J34" s="6">
-        <f t="shared" si="11"/>
-        <v>1.8065929350925032</v>
+      <c r="J34" s="5" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
@@ -4284,19 +4210,19 @@
         <v>4367214</v>
       </c>
       <c r="G42" s="3">
-        <f t="shared" ref="G42:G46" si="12">C42/B42</f>
+        <f t="shared" ref="G42:G46" si="16">C42/B42</f>
         <v>0.91550953580239969</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" ref="H42:H46" si="13">D42/B42</f>
+        <f t="shared" ref="H42:H46" si="17">D42/B42</f>
         <v>0.86825919820597031</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" ref="I42:I46" si="14">E42/B42</f>
+        <f t="shared" ref="I42:I46" si="18">E42/B42</f>
         <v>0.90117688580484256</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" ref="J42:J46" si="15">F42/B42</f>
+        <f t="shared" ref="J42:J46" si="19">F42/B42</f>
         <v>0.97429760645079677</v>
       </c>
     </row>
@@ -4320,19 +4246,19 @@
         <v>4479895</v>
       </c>
       <c r="G43" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.96932551880980444</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.98763347412772062</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.98229439747208147</v>
       </c>
       <c r="J43" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.99943601931366144</v>
       </c>
     </row>
@@ -4356,19 +4282,19 @@
         <v>4479895</v>
       </c>
       <c r="G44" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.99913551219954033</v>
       </c>
       <c r="H44" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.99943601931366144</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.9991593832175143</v>
       </c>
       <c r="J44" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.99943601931366144</v>
       </c>
     </row>
@@ -4392,19 +4318,19 @@
         <v>4479895</v>
       </c>
       <c r="G45" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.99916317580915504</v>
       </c>
       <c r="H45" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.99943601931366144</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.99916317580915504</v>
       </c>
       <c r="J45" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.99943601931366144</v>
       </c>
     </row>
@@ -4428,135 +4354,135 @@
         <v>4479895</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.99916317580915504</v>
       </c>
       <c r="H46" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.99943601931366144</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.99916317580915504</v>
       </c>
       <c r="J46" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.99943601931366144</v>
       </c>
     </row>
     <row r="47" spans="1:10">
-      <c r="G47" s="5" t="s">
+      <c r="G47" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="G48" s="6">
+      <c r="G48" s="5">
         <f>G41/G41</f>
         <v>1</v>
       </c>
-      <c r="H48" s="6">
+      <c r="H48" s="5">
         <f>H41/G41</f>
         <v>0.90872847666945433</v>
       </c>
-      <c r="I48" s="6">
+      <c r="I48" s="5">
         <f>I41/G41</f>
         <v>1.0743698136840456</v>
       </c>
-      <c r="J48" s="6">
+      <c r="J48" s="5">
         <f>J41/G41</f>
         <v>1.1487306260702679</v>
       </c>
     </row>
     <row r="49" spans="1:10">
-      <c r="G49" s="6">
-        <f t="shared" ref="G49:G53" si="16">G42/G42</f>
-        <v>1</v>
-      </c>
-      <c r="H49" s="6">
-        <f t="shared" ref="H49:H53" si="17">H42/G42</f>
+      <c r="G49" s="5">
+        <f t="shared" ref="G49:G53" si="20">G42/G42</f>
+        <v>1</v>
+      </c>
+      <c r="H49" s="5">
+        <f t="shared" ref="H49:H53" si="21">H42/G42</f>
         <v>0.94838902736822206</v>
       </c>
-      <c r="I49" s="6">
-        <f t="shared" ref="I49:I53" si="18">I42/G42</f>
+      <c r="I49" s="5">
+        <f t="shared" ref="I49:I53" si="22">I42/G42</f>
         <v>0.98434461964943354</v>
       </c>
-      <c r="J49" s="6">
-        <f t="shared" ref="J49:J53" si="19">J42/G42</f>
+      <c r="J49" s="5">
+        <f t="shared" ref="J49:J53" si="23">J42/G42</f>
         <v>1.0642134989854279</v>
       </c>
     </row>
     <row r="50" spans="1:10">
-      <c r="G50" s="6">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="H50" s="6">
-        <f t="shared" si="17"/>
+      <c r="G50" s="5">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="H50" s="5">
+        <f t="shared" si="21"/>
         <v>1.0188873138720167</v>
       </c>
-      <c r="I50" s="6">
-        <f t="shared" si="18"/>
+      <c r="I50" s="5">
+        <f t="shared" si="22"/>
         <v>1.0133792811708919</v>
       </c>
-      <c r="J50" s="6">
-        <f t="shared" si="19"/>
+      <c r="J50" s="5">
+        <f t="shared" si="23"/>
         <v>1.0310633527329689</v>
       </c>
     </row>
     <row r="51" spans="1:10">
-      <c r="G51" s="6">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="H51" s="6">
-        <f t="shared" si="17"/>
+      <c r="G51" s="5">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="H51" s="5">
+        <f t="shared" si="21"/>
         <v>1.0003007671236304</v>
       </c>
-      <c r="I51" s="6">
-        <f t="shared" si="18"/>
+      <c r="I51" s="5">
+        <f t="shared" si="22"/>
         <v>1.000023891672033</v>
       </c>
-      <c r="J51" s="6">
-        <f t="shared" si="19"/>
+      <c r="J51" s="5">
+        <f t="shared" si="23"/>
         <v>1.0003007671236304</v>
       </c>
     </row>
     <row r="52" spans="1:10">
-      <c r="G52" s="6">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="H52" s="6">
-        <f t="shared" si="17"/>
+      <c r="G52" s="5">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="H52" s="5">
+        <f t="shared" si="21"/>
         <v>1.0002730720177768</v>
       </c>
-      <c r="I52" s="6">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="J52" s="6">
-        <f t="shared" si="19"/>
+      <c r="I52" s="5">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="J52" s="5">
+        <f t="shared" si="23"/>
         <v>1.0002730720177768</v>
       </c>
     </row>
     <row r="53" spans="1:10">
-      <c r="G53" s="6">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="H53" s="6">
-        <f t="shared" si="17"/>
+      <c r="G53" s="5">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="H53" s="5">
+        <f t="shared" si="21"/>
         <v>1.0002730720177768</v>
       </c>
-      <c r="I53" s="6">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="J53" s="6">
-        <f t="shared" si="19"/>
+      <c r="I53" s="5">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="J53" s="5">
+        <f t="shared" si="23"/>
         <v>1.0002730720177768</v>
       </c>
     </row>
@@ -4620,19 +4546,19 @@
         <v>11.6172</v>
       </c>
       <c r="G57" s="3">
-        <f>C57/A57</f>
+        <f t="shared" ref="G57:G62" si="24">C57/A57</f>
         <v>1</v>
       </c>
       <c r="H57" s="3">
-        <f>D57/A57</f>
+        <f t="shared" ref="H57:H62" si="25">D57/A57</f>
         <v>1</v>
       </c>
       <c r="I57" s="3">
-        <f>E57/A57</f>
+        <f t="shared" ref="I57:I62" si="26">E57/A57</f>
         <v>1</v>
       </c>
       <c r="J57" s="3">
-        <f>F57/A57</f>
+        <f t="shared" ref="J57:J62" si="27">F57/A57</f>
         <v>0.72607500000000003</v>
       </c>
     </row>
@@ -4653,19 +4579,19 @@
         <v>22.3828</v>
       </c>
       <c r="G58" s="3">
-        <f>C58/A58</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="H58" s="3">
-        <f>D58/A58</f>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="I58" s="3">
-        <f>E58/A58</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="J58" s="3">
-        <f>F58/A58</f>
+        <f t="shared" si="27"/>
         <v>0.69946249999999999</v>
       </c>
     </row>
@@ -4686,19 +4612,19 @@
         <v>26.3047</v>
       </c>
       <c r="G59" s="3">
-        <f>C59/A59</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="H59" s="3">
-        <f>D59/A59</f>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="I59" s="3">
-        <f>E59/A59</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="J59" s="3">
-        <f>F59/A59</f>
+        <f t="shared" si="27"/>
         <v>0.41101093750000001</v>
       </c>
     </row>
@@ -4719,19 +4645,19 @@
         <v>26.3047</v>
       </c>
       <c r="G60" s="3">
-        <f>C60/A60</f>
+        <f t="shared" si="24"/>
         <v>0.9140625</v>
       </c>
       <c r="H60" s="3">
-        <f>D60/A60</f>
+        <f t="shared" si="25"/>
         <v>0.6171875</v>
       </c>
       <c r="I60" s="3">
-        <f>E60/A60</f>
+        <f t="shared" si="26"/>
         <v>0.90600781249999995</v>
       </c>
       <c r="J60" s="3">
-        <f>F60/A60</f>
+        <f t="shared" si="27"/>
         <v>0.20550546875</v>
       </c>
     </row>
@@ -4752,19 +4678,19 @@
         <v>26.3047</v>
       </c>
       <c r="G61" s="3">
-        <f>C61/A61</f>
+        <f t="shared" si="24"/>
         <v>0.45788671874999998</v>
       </c>
       <c r="H61" s="3">
-        <f>D61/A61</f>
+        <f t="shared" si="25"/>
         <v>0.30859375</v>
       </c>
       <c r="I61" s="3">
-        <f>E61/A61</f>
+        <f t="shared" si="26"/>
         <v>0.45342968750000001</v>
       </c>
       <c r="J61" s="3">
-        <f>F61/A61</f>
+        <f t="shared" si="27"/>
         <v>0.102752734375</v>
       </c>
     </row>
@@ -4785,19 +4711,19 @@
         <v>26.3047</v>
       </c>
       <c r="G62" s="3">
-        <f>C62/A62</f>
+        <f t="shared" si="24"/>
         <v>0.22894335937499999</v>
       </c>
       <c r="H62" s="3">
-        <f>D62/A62</f>
+        <f t="shared" si="25"/>
         <v>0.154296875</v>
       </c>
       <c r="I62" s="3">
-        <f>E62/A62</f>
+        <f t="shared" si="26"/>
         <v>0.22671484375000001</v>
       </c>
       <c r="J62" s="3">
-        <f>F62/A62</f>
+        <f t="shared" si="27"/>
         <v>5.1376367187500001E-2</v>
       </c>
     </row>
@@ -4807,110 +4733,110 @@
       </c>
     </row>
     <row r="64" spans="1:10">
-      <c r="G64" s="6">
+      <c r="G64" s="5">
         <f>G57/G57</f>
         <v>1</v>
       </c>
-      <c r="H64" s="6">
+      <c r="H64" s="5">
         <f>G57/H57</f>
         <v>1</v>
       </c>
-      <c r="I64" s="6">
+      <c r="I64" s="5">
         <f>G57/I57</f>
         <v>1</v>
       </c>
-      <c r="J64" s="6">
+      <c r="J64" s="5">
         <f>G57/J57</f>
         <v>1.3772681885480149</v>
       </c>
     </row>
     <row r="65" spans="7:10">
-      <c r="G65" s="6">
-        <f t="shared" ref="G65:G69" si="20">G58/G58</f>
-        <v>1</v>
-      </c>
-      <c r="H65" s="6">
-        <f t="shared" ref="H65:H69" si="21">G58/H58</f>
-        <v>1</v>
-      </c>
-      <c r="I65" s="6">
-        <f t="shared" ref="I65:I69" si="22">G58/I58</f>
-        <v>1</v>
-      </c>
-      <c r="J65" s="6">
-        <f t="shared" ref="J65:J69" si="23">G58/J58</f>
+      <c r="G65" s="5">
+        <f t="shared" ref="G65:G69" si="28">G58/G58</f>
+        <v>1</v>
+      </c>
+      <c r="H65" s="5">
+        <f t="shared" ref="H65:H69" si="29">G58/H58</f>
+        <v>1</v>
+      </c>
+      <c r="I65" s="5">
+        <f t="shared" ref="I65:I69" si="30">G58/I58</f>
+        <v>1</v>
+      </c>
+      <c r="J65" s="5">
+        <f t="shared" ref="J65:J69" si="31">G58/J58</f>
         <v>1.4296692102864701</v>
       </c>
     </row>
     <row r="66" spans="7:10">
-      <c r="G66" s="6">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="H66" s="6">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
-      <c r="I66" s="6">
-        <f t="shared" si="22"/>
-        <v>1</v>
-      </c>
-      <c r="J66" s="6">
-        <f t="shared" si="23"/>
+      <c r="G66" s="5">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="H66" s="5">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="I66" s="5">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="J66" s="5">
+        <f t="shared" si="31"/>
         <v>2.4330252768516654</v>
       </c>
     </row>
     <row r="67" spans="7:10">
-      <c r="G67" s="6">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="H67" s="6">
-        <f t="shared" si="21"/>
+      <c r="G67" s="5">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="H67" s="5">
+        <f t="shared" si="29"/>
         <v>1.481012658227848</v>
       </c>
-      <c r="I67" s="6">
-        <f t="shared" si="22"/>
+      <c r="I67" s="5">
+        <f t="shared" si="30"/>
         <v>1.0088903068923591</v>
       </c>
-      <c r="J67" s="6">
-        <f t="shared" si="23"/>
+      <c r="J67" s="5">
+        <f t="shared" si="31"/>
         <v>4.4478743342444504</v>
       </c>
     </row>
     <row r="68" spans="7:10">
-      <c r="G68" s="6">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="H68" s="6">
-        <f t="shared" si="21"/>
+      <c r="G68" s="5">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="H68" s="5">
+        <f t="shared" si="29"/>
         <v>1.4837848101265823</v>
       </c>
-      <c r="I68" s="6">
-        <f t="shared" si="22"/>
+      <c r="I68" s="5">
+        <f t="shared" si="30"/>
         <v>1.0098295973397198</v>
       </c>
-      <c r="J68" s="6">
-        <f t="shared" si="23"/>
+      <c r="J68" s="5">
+        <f t="shared" si="31"/>
         <v>4.4561998426136773</v>
       </c>
     </row>
     <row r="69" spans="7:10">
-      <c r="G69" s="6">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="H69" s="6">
-        <f t="shared" si="21"/>
+      <c r="G69" s="5">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="H69" s="5">
+        <f t="shared" si="29"/>
         <v>1.4837848101265823</v>
       </c>
-      <c r="I69" s="6">
-        <f t="shared" si="22"/>
+      <c r="I69" s="5">
+        <f t="shared" si="30"/>
         <v>1.0098295973397198</v>
       </c>
-      <c r="J69" s="6">
-        <f t="shared" si="23"/>
+      <c r="J69" s="5">
+        <f t="shared" si="31"/>
         <v>4.4561998426136773</v>
       </c>
     </row>
@@ -4920,7 +4846,6 @@
     <mergeCell ref="G47:J47"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4933,7 +4858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated data and graphs for new bisort.pool trace
</commit_message>
<xml_diff>
--- a/documents/data/cache-config.xlsx
+++ b/documents/data/cache-config.xlsx
@@ -277,10 +277,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$13:$G$17</c:f>
+              <c:f>Sheet1!$G$13:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -294,6 +294,9 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -343,10 +346,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$13:$H$17</c:f>
+              <c:f>Sheet1!$H$13:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.968642352183527</c:v>
                 </c:pt>
@@ -360,6 +363,9 @@
                   <c:v>1.002501855976244</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.001265450483071</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.001265450483071</c:v>
                 </c:pt>
               </c:numCache>
@@ -409,10 +415,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$13:$I$17</c:f>
+              <c:f>Sheet1!$I$13:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.12900956955952</c:v>
                 </c:pt>
@@ -426,6 +432,9 @@
                   <c:v>1.001186999917512</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -482,10 +491,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$13:$J$17</c:f>
+              <c:f>Sheet1!$J$13:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.151292819571437</c:v>
                 </c:pt>
@@ -499,6 +508,9 @@
                   <c:v>1.002501855976244</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.001265450483071</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.001265450483071</c:v>
                 </c:pt>
               </c:numCache>
@@ -528,6 +540,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2115926392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -539,6 +561,7 @@
         <c:axId val="2115926392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -715,10 +738,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$29:$G$33</c:f>
+              <c:f>Sheet1!$G$29:$G$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -732,6 +755,9 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -781,10 +807,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$29:$H$33</c:f>
+              <c:f>Sheet1!$H$29:$H$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -798,6 +824,9 @@
                   <c:v>1.573825</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.6</c:v>
                 </c:pt>
               </c:numCache>
@@ -847,10 +876,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$29:$I$33</c:f>
+              <c:f>Sheet1!$I$29:$I$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.031738866892789</c:v>
                 </c:pt>
@@ -864,6 +893,9 @@
                   <c:v>1.187098112424808</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1.206215780694893</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.206215780694893</c:v>
                 </c:pt>
               </c:numCache>
@@ -920,10 +952,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$29:$J$33</c:f>
+              <c:f>Sheet1!$J$29:$J$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0307020369249</c:v>
                 </c:pt>
@@ -937,6 +969,9 @@
                   <c:v>2.25146141314941</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>2.287311319153194</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>2.287311319153194</c:v>
                 </c:pt>
               </c:numCache>
@@ -966,6 +1001,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2115837016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1416,6 +1461,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2121861496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1427,6 +1482,7 @@
         <c:axId val="2121861496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1866,6 +1922,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="2115941752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -3339,7 +3405,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3954,18 +4020,22 @@
       <c r="C27" s="4">
         <v>128</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="4">
+        <v>80</v>
+      </c>
       <c r="E27" s="4">
         <v>106.117</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4">
+        <v>55.960900000000002</v>
+      </c>
       <c r="G27" s="3">
         <f t="shared" si="8"/>
         <v>0.25</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.15625</v>
       </c>
       <c r="I27" s="3">
         <f t="shared" si="10"/>
@@ -3973,7 +4043,7 @@
       </c>
       <c r="J27" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.1092986328125</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -4076,17 +4146,17 @@
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="H34" s="5" t="e">
+      <c r="H34" s="5">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>1.6</v>
       </c>
       <c r="I34" s="5">
         <f t="shared" si="14"/>
         <v>1.2062157806948932</v>
       </c>
-      <c r="J34" s="5" t="e">
+      <c r="J34" s="5">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
+        <v>2.2873113191531944</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -4858,8 +4928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J76" sqref="J76"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
more data, better graphs, clean up
</commit_message>
<xml_diff>
--- a/documents/data/cache-config.xlsx
+++ b/documents/data/cache-config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="27">
   <si>
     <t>SIZE (KB)</t>
   </si>
@@ -90,6 +90,18 @@
   <si>
     <t>256KB</t>
   </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>Benchmark Averages</t>
+  </si>
+  <si>
+    <t>Compression</t>
+  </si>
 </sst>
 </file>
 
@@ -145,8 +157,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -171,17 +195,29 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,11 +562,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2078396760"/>
-        <c:axId val="2115926392"/>
+        <c:axId val="2039699832"/>
+        <c:axId val="2039702920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078396760"/>
+        <c:axId val="2039699832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -550,7 +586,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115926392"/>
+        <c:crossAx val="2039702920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -558,7 +594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115926392"/>
+        <c:axId val="2039702920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -604,7 +640,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078396760"/>
+        <c:crossAx val="2039699832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -987,11 +1023,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115818360"/>
-        <c:axId val="2115837016"/>
+        <c:axId val="2046704472"/>
+        <c:axId val="2046707560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115818360"/>
+        <c:axId val="2046704472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,7 +1047,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115837016"/>
+        <c:crossAx val="2046707560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1019,7 +1055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115837016"/>
+        <c:axId val="2046707560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,7 +1100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115818360"/>
+        <c:crossAx val="2046704472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1447,11 +1483,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121858440"/>
-        <c:axId val="2121861496"/>
+        <c:axId val="2046759816"/>
+        <c:axId val="2046762904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121858440"/>
+        <c:axId val="2046759816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,7 +1507,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121861496"/>
+        <c:crossAx val="2046762904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1479,7 +1515,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121861496"/>
+        <c:axId val="2046762904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -1525,7 +1561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121858440"/>
+        <c:crossAx val="2046759816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1908,11 +1944,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115938696"/>
-        <c:axId val="2115941752"/>
+        <c:axId val="2045775416"/>
+        <c:axId val="2045772312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115938696"/>
+        <c:axId val="2045775416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1932,7 +1968,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2115941752"/>
+        <c:crossAx val="2045772312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1940,7 +1976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115941752"/>
+        <c:axId val="2045772312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1985,7 +2021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115938696"/>
+        <c:crossAx val="2045775416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2052,15 +2088,15 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Normalized Hit Ratio for LLU Benchmark by Cache Size</a:t>
+              <a:t>Normalized Hit Ratio for Micro-Benchmarks by Cache Size</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -2119,10 +2155,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$48:$G$51</c:f>
+              <c:f>Sheet1!$C$108:$C$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2133,6 +2169,12 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2182,21 +2224,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$48:$H$51</c:f>
+              <c:f>Sheet1!$D$108:$D$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.908728476669454</c:v>
+                  <c:v>1.024006030546149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.948389027368222</c:v>
+                  <c:v>1.03173787796673</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.018887313872017</c:v>
+                  <c:v>1.032341503999978</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.00030076712363</c:v>
+                  <c:v>1.000940434625904</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.000519067759562</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.000519067759562</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2245,21 +2293,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$48:$I$51</c:f>
+              <c:f>Sheet1!$E$108:$E$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.074369813684046</c:v>
+                  <c:v>1.062201776451157</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.984344619649433</c:v>
+                  <c:v>1.012846415231759</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.013379281170892</c:v>
+                  <c:v>1.031649815157421</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.000023891672033</c:v>
+                  <c:v>1.000403630529848</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2315,21 +2369,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$48:$J$51</c:f>
+              <c:f>Sheet1!$F$108:$F$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.148730626070268</c:v>
+                  <c:v>1.192692455996015</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.064213498985428</c:v>
+                  <c:v>1.115564732098642</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.031063352732969</c:v>
+                  <c:v>1.0450146814442</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.00030076712363</c:v>
+                  <c:v>1.000940434625904</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.000519067759562</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.000519067759562</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2344,21 +2404,50 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2115844840"/>
-        <c:axId val="2115847896"/>
+        <c:axId val="2077281000"/>
+        <c:axId val="2077284056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2115844840"/>
+        <c:axId val="2077281000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Cache Capacity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115847896"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2077284056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2366,9 +2455,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115847896"/>
+        <c:axId val="2077284056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.7"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2390,17 +2480,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Normalized</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
                   <a:t> Hit Ratio</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1600"/>
+                <a:endParaRPr lang="en-US" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2411,7 +2501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115844840"/>
+        <c:crossAx val="2077281000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2422,8 +2512,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.209131952081409"/>
-          <c:y val="0.903729065600546"/>
+          <c:x val="0.212856346867256"/>
+          <c:y val="0.872769313278564"/>
           <c:w val="0.579086496869455"/>
           <c:h val="0.0645752841987999"/>
         </c:manualLayout>
@@ -2474,19 +2564,21 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr lIns="2" anchor="ctr" anchorCtr="1">
+            <a:spAutoFit/>
+          </a:bodyPr>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Normalized Compression Ratio for LLU Benchmark by Cache Size</a:t>
+              <a:t>Normalized Compression Ratio for Micro-Benchmarks by Cache Size</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -2545,10 +2637,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$64:$G$67</c:f>
+              <c:f>Sheet1!$G$108:$G$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2559,6 +2651,12 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2608,10 +2706,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$64:$H$67</c:f>
+              <c:f>Sheet1!$H$108:$H$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2619,10 +2717,16 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1.002955665024631</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.481012658227848</c:v>
+                  <c:v>1.428264654387162</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.437995554568013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.437995554568013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2671,21 +2775,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$64:$I$67</c:f>
+              <c:f>Sheet1!$I$108:$I$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1.010742201554985</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1.011007198126131</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1.007017993933972</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.008890306892359</c:v>
+                  <c:v>1.065329473105723</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.07208167272349</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.07208167272349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2741,21 +2851,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$64:$J$67</c:f>
+              <c:f>Sheet1!$J$108:$J$113</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.377268188548015</c:v>
+                  <c:v>1.223276577729992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.42966921028647</c:v>
+                  <c:v>1.236958602412401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.433025276851665</c:v>
+                  <c:v>1.67733345210052</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.44787433424445</c:v>
+                  <c:v>2.825401148404991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.840244531232193</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.840244531232193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2770,21 +2886,50 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2123561176"/>
-        <c:axId val="2123564232"/>
+        <c:axId val="2077328600"/>
+        <c:axId val="2077331656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2123561176"/>
+        <c:axId val="2077328600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Cache Capacity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123564232"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2077331656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2792,7 +2937,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123564232"/>
+        <c:axId val="2077331656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2816,17 +2961,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1200"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Normalized</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
                   <a:t> Compression Ratio</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1600"/>
+                <a:endParaRPr lang="en-US" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2837,7 +2982,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123561176"/>
+        <c:crossAx val="2077328600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2849,7 +2994,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.184923385973401"/>
-          <c:y val="0.906825040832744"/>
+          <c:y val="0.878961263742961"/>
           <c:w val="0.62750362908547"/>
           <c:h val="0.0645752841987999"/>
         </c:manualLayout>
@@ -3402,10 +3547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4820,7 +4965,7 @@
         <v>1.3772681885480149</v>
       </c>
     </row>
-    <row r="65" spans="7:10">
+    <row r="65" spans="1:10">
       <c r="G65" s="5">
         <f t="shared" ref="G65:G69" si="28">G58/G58</f>
         <v>1</v>
@@ -4838,7 +4983,7 @@
         <v>1.4296692102864701</v>
       </c>
     </row>
-    <row r="66" spans="7:10">
+    <row r="66" spans="1:10">
       <c r="G66" s="5">
         <f t="shared" si="28"/>
         <v>1</v>
@@ -4856,7 +5001,7 @@
         <v>2.4330252768516654</v>
       </c>
     </row>
-    <row r="67" spans="7:10">
+    <row r="67" spans="1:10">
       <c r="G67" s="5">
         <f t="shared" si="28"/>
         <v>1</v>
@@ -4874,7 +5019,7 @@
         <v>4.4478743342444504</v>
       </c>
     </row>
-    <row r="68" spans="7:10">
+    <row r="68" spans="1:10">
       <c r="G68" s="5">
         <f t="shared" si="28"/>
         <v>1</v>
@@ -4892,7 +5037,7 @@
         <v>4.4561998426136773</v>
       </c>
     </row>
-    <row r="69" spans="7:10">
+    <row r="69" spans="1:10">
       <c r="G69" s="5">
         <f t="shared" si="28"/>
         <v>1</v>
@@ -4910,12 +5055,1021 @@
         <v>4.4561998426136773</v>
       </c>
     </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76">
+        <v>25054991</v>
+      </c>
+      <c r="C76" s="4">
+        <v>19596217</v>
+      </c>
+      <c r="D76" s="4">
+        <v>23410567</v>
+      </c>
+      <c r="E76" s="4">
+        <v>19267509</v>
+      </c>
+      <c r="F76" s="4">
+        <v>25045022</v>
+      </c>
+      <c r="G76" s="3">
+        <f>C76/B76</f>
+        <v>0.782128279351607</v>
+      </c>
+      <c r="H76" s="3">
+        <f>D76/B76</f>
+        <v>0.93436740807450303</v>
+      </c>
+      <c r="I76" s="3">
+        <f>E76/B76</f>
+        <v>0.76900881744479577</v>
+      </c>
+      <c r="J76" s="3">
+        <f>F76/B76</f>
+        <v>0.99960211520331421</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77">
+        <v>25054991</v>
+      </c>
+      <c r="C77" s="4">
+        <v>21154503</v>
+      </c>
+      <c r="D77" s="4">
+        <v>24159741</v>
+      </c>
+      <c r="E77" s="4">
+        <v>20686732</v>
+      </c>
+      <c r="F77" s="4">
+        <v>25050325</v>
+      </c>
+      <c r="G77" s="3">
+        <f t="shared" ref="G77:G81" si="32">C77/B77</f>
+        <v>0.84432291354644673</v>
+      </c>
+      <c r="H77" s="3">
+        <f t="shared" ref="H77:H81" si="33">D77/B77</f>
+        <v>0.96426859622499961</v>
+      </c>
+      <c r="I77" s="3">
+        <f t="shared" ref="I77:I81" si="34">E77/B77</f>
+        <v>0.82565314032641246</v>
+      </c>
+      <c r="J77" s="3">
+        <f t="shared" ref="J77:J81" si="35">F77/B77</f>
+        <v>0.99981376963974966</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" t="s">
+        <v>15</v>
+      </c>
+      <c r="B78">
+        <v>25054991</v>
+      </c>
+      <c r="C78" s="4">
+        <v>23869137</v>
+      </c>
+      <c r="D78" s="4">
+        <v>25051686</v>
+      </c>
+      <c r="E78" s="4">
+        <v>25048207</v>
+      </c>
+      <c r="F78" s="4">
+        <v>25052958</v>
+      </c>
+      <c r="G78" s="3">
+        <f t="shared" si="32"/>
+        <v>0.95266994907322056</v>
+      </c>
+      <c r="H78" s="3">
+        <f t="shared" si="33"/>
+        <v>0.99986809015417333</v>
+      </c>
+      <c r="I78" s="3">
+        <f t="shared" si="34"/>
+        <v>0.99972923558423943</v>
+      </c>
+      <c r="J78" s="3">
+        <f t="shared" si="35"/>
+        <v>0.99991885848212836</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79">
+        <v>25054991</v>
+      </c>
+      <c r="C79" s="4">
+        <v>25052490</v>
+      </c>
+      <c r="D79" s="4">
+        <v>25052958</v>
+      </c>
+      <c r="E79" s="4">
+        <v>25052490</v>
+      </c>
+      <c r="F79" s="4">
+        <v>25052958</v>
+      </c>
+      <c r="G79" s="3">
+        <f t="shared" si="32"/>
+        <v>0.99990017956901278</v>
+      </c>
+      <c r="H79" s="3">
+        <f t="shared" si="33"/>
+        <v>0.99991885848212836</v>
+      </c>
+      <c r="I79" s="3">
+        <f t="shared" si="34"/>
+        <v>0.99990017956901278</v>
+      </c>
+      <c r="J79" s="3">
+        <f t="shared" si="35"/>
+        <v>0.99991885848212836</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" t="s">
+        <v>17</v>
+      </c>
+      <c r="B80">
+        <v>25054991</v>
+      </c>
+      <c r="C80" s="4">
+        <v>25052490</v>
+      </c>
+      <c r="D80" s="4">
+        <v>25052958</v>
+      </c>
+      <c r="E80" s="4">
+        <v>25052490</v>
+      </c>
+      <c r="F80" s="4">
+        <v>25052958</v>
+      </c>
+      <c r="G80" s="3">
+        <f t="shared" si="32"/>
+        <v>0.99990017956901278</v>
+      </c>
+      <c r="H80" s="3">
+        <f t="shared" si="33"/>
+        <v>0.99991885848212836</v>
+      </c>
+      <c r="I80" s="3">
+        <f t="shared" si="34"/>
+        <v>0.99990017956901278</v>
+      </c>
+      <c r="J80" s="3">
+        <f t="shared" si="35"/>
+        <v>0.99991885848212836</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81">
+        <v>25054991</v>
+      </c>
+      <c r="C81" s="4">
+        <v>25052490</v>
+      </c>
+      <c r="D81" s="4">
+        <v>25052958</v>
+      </c>
+      <c r="E81" s="4">
+        <v>25052490</v>
+      </c>
+      <c r="F81" s="4">
+        <v>25052958</v>
+      </c>
+      <c r="G81" s="3">
+        <f t="shared" si="32"/>
+        <v>0.99990017956901278</v>
+      </c>
+      <c r="H81" s="3">
+        <f t="shared" si="33"/>
+        <v>0.99991885848212836</v>
+      </c>
+      <c r="I81" s="3">
+        <f t="shared" si="34"/>
+        <v>0.99990017956901278</v>
+      </c>
+      <c r="J81" s="3">
+        <f t="shared" si="35"/>
+        <v>0.99991885848212836</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="G82" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="G83" s="5">
+        <f>G76/G76</f>
+        <v>1</v>
+      </c>
+      <c r="H83" s="5">
+        <f>H76/G76</f>
+        <v>1.1946472627854652</v>
+      </c>
+      <c r="I83" s="5">
+        <f>I76/G76</f>
+        <v>0.98322594610990488</v>
+      </c>
+      <c r="J83" s="5">
+        <f>J76/G76</f>
+        <v>1.2780539223463387</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="G84" s="5">
+        <f t="shared" ref="G84:G88" si="36">G77/G77</f>
+        <v>1</v>
+      </c>
+      <c r="H84" s="5">
+        <f t="shared" ref="H84:H88" si="37">H77/G77</f>
+        <v>1.1420613852284782</v>
+      </c>
+      <c r="I84" s="5">
+        <f t="shared" ref="I84:I88" si="38">I77/G77</f>
+        <v>0.97788787569247082</v>
+      </c>
+      <c r="J84" s="5">
+        <f t="shared" ref="J84:J88" si="39">J77/G77</f>
+        <v>1.1841604125608622</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="G85" s="5">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="H85" s="5">
+        <f t="shared" si="37"/>
+        <v>1.0495430144793254</v>
+      </c>
+      <c r="I85" s="5">
+        <f t="shared" si="38"/>
+        <v>1.0493972614091578</v>
+      </c>
+      <c r="J85" s="5">
+        <f t="shared" si="39"/>
+        <v>1.0495963050528387</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="G86" s="5">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="H86" s="5">
+        <f t="shared" si="37"/>
+        <v>1.0000186807778388</v>
+      </c>
+      <c r="I86" s="5">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="J86" s="5">
+        <f t="shared" si="39"/>
+        <v>1.0000186807778388</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="G87" s="5">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="H87" s="5">
+        <f t="shared" si="37"/>
+        <v>1.0000186807778388</v>
+      </c>
+      <c r="I87" s="5">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="J87" s="5">
+        <f t="shared" si="39"/>
+        <v>1.0000186807778388</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="G88" s="5">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="H88" s="5">
+        <f t="shared" si="37"/>
+        <v>1.0000186807778388</v>
+      </c>
+      <c r="I88" s="5">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="J88" s="5">
+        <f t="shared" si="39"/>
+        <v>1.0000186807778388</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92">
+        <v>16</v>
+      </c>
+      <c r="C92" s="4">
+        <v>16</v>
+      </c>
+      <c r="D92" s="4">
+        <v>16</v>
+      </c>
+      <c r="E92" s="4">
+        <v>15.9922</v>
+      </c>
+      <c r="F92" s="4">
+        <v>12.6797</v>
+      </c>
+      <c r="G92" s="3">
+        <f t="shared" ref="G92:G97" si="40">C92/A92</f>
+        <v>1</v>
+      </c>
+      <c r="H92" s="3">
+        <f t="shared" ref="H92:H97" si="41">D92/A92</f>
+        <v>1</v>
+      </c>
+      <c r="I92" s="3">
+        <f t="shared" ref="I92:I97" si="42">E92/A92</f>
+        <v>0.99951250000000003</v>
+      </c>
+      <c r="J92" s="3">
+        <f t="shared" ref="J92:J97" si="43">F92/A92</f>
+        <v>0.79248125000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93">
+        <v>32</v>
+      </c>
+      <c r="C93" s="4">
+        <v>32</v>
+      </c>
+      <c r="D93" s="4">
+        <v>32</v>
+      </c>
+      <c r="E93" s="4">
+        <v>31.9922</v>
+      </c>
+      <c r="F93" s="4">
+        <v>25.468800000000002</v>
+      </c>
+      <c r="G93" s="3">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+      <c r="H93" s="3">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="I93" s="3">
+        <f t="shared" si="42"/>
+        <v>0.99975625000000001</v>
+      </c>
+      <c r="J93" s="3">
+        <f t="shared" si="43"/>
+        <v>0.79590000000000005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94">
+        <v>64</v>
+      </c>
+      <c r="C94" s="4">
+        <v>64</v>
+      </c>
+      <c r="D94" s="4">
+        <v>63.4375</v>
+      </c>
+      <c r="E94" s="4">
+        <v>63.984400000000001</v>
+      </c>
+      <c r="F94" s="4">
+        <v>43.976599999999998</v>
+      </c>
+      <c r="G94" s="3">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+      <c r="H94" s="3">
+        <f t="shared" si="41"/>
+        <v>0.9912109375</v>
+      </c>
+      <c r="I94" s="3">
+        <f t="shared" si="42"/>
+        <v>0.99975625000000001</v>
+      </c>
+      <c r="J94" s="3">
+        <f t="shared" si="43"/>
+        <v>0.68713437499999996</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95">
+        <v>128</v>
+      </c>
+      <c r="C95">
+        <v>78.156199999999998</v>
+      </c>
+      <c r="D95" s="4">
+        <v>63.531199999999998</v>
+      </c>
+      <c r="E95" s="4">
+        <v>78.140600000000006</v>
+      </c>
+      <c r="F95" s="4">
+        <v>43.976599999999998</v>
+      </c>
+      <c r="G95" s="3">
+        <f>E95/A95</f>
+        <v>0.61047343750000005</v>
+      </c>
+      <c r="H95" s="3">
+        <f t="shared" si="41"/>
+        <v>0.49633749999999999</v>
+      </c>
+      <c r="I95" s="3">
+        <f>E95/A95</f>
+        <v>0.61047343750000005</v>
+      </c>
+      <c r="J95" s="3">
+        <f t="shared" si="43"/>
+        <v>0.34356718749999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96">
+        <v>256</v>
+      </c>
+      <c r="C96" s="4">
+        <v>78.156199999999998</v>
+      </c>
+      <c r="D96" s="4">
+        <v>63.531199999999998</v>
+      </c>
+      <c r="E96" s="4">
+        <v>78.140600000000006</v>
+      </c>
+      <c r="F96" s="4">
+        <v>43.976599999999998</v>
+      </c>
+      <c r="G96" s="3">
+        <f t="shared" si="40"/>
+        <v>0.30529765624999999</v>
+      </c>
+      <c r="H96" s="3">
+        <f t="shared" si="41"/>
+        <v>0.24816874999999999</v>
+      </c>
+      <c r="I96" s="3">
+        <f t="shared" si="42"/>
+        <v>0.30523671875000002</v>
+      </c>
+      <c r="J96" s="3">
+        <f t="shared" si="43"/>
+        <v>0.17178359374999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97">
+        <v>512</v>
+      </c>
+      <c r="C97" s="4">
+        <v>78.156199999999998</v>
+      </c>
+      <c r="D97" s="4">
+        <v>63.531199999999998</v>
+      </c>
+      <c r="E97" s="4">
+        <v>78.140600000000006</v>
+      </c>
+      <c r="F97" s="4">
+        <v>43.976599999999998</v>
+      </c>
+      <c r="G97" s="3">
+        <f t="shared" si="40"/>
+        <v>0.152648828125</v>
+      </c>
+      <c r="H97" s="3">
+        <f t="shared" si="41"/>
+        <v>0.124084375</v>
+      </c>
+      <c r="I97" s="3">
+        <f t="shared" si="42"/>
+        <v>0.15261835937500001</v>
+      </c>
+      <c r="J97" s="3">
+        <f t="shared" si="43"/>
+        <v>8.5891796874999995E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="G98" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="G99" s="5">
+        <f>G92/G92</f>
+        <v>1</v>
+      </c>
+      <c r="H99" s="5">
+        <f>G92/H92</f>
+        <v>1</v>
+      </c>
+      <c r="I99" s="5">
+        <f>G92/I92</f>
+        <v>1.0004877377721639</v>
+      </c>
+      <c r="J99" s="5">
+        <f>G92/J92</f>
+        <v>1.2618595077170596</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="G100" s="5">
+        <f t="shared" ref="G100:G104" si="44">G93/G93</f>
+        <v>1</v>
+      </c>
+      <c r="H100" s="5">
+        <f t="shared" ref="H100:H104" si="45">G93/H93</f>
+        <v>1</v>
+      </c>
+      <c r="I100" s="5">
+        <f t="shared" ref="I100:I104" si="46">G93/I93</f>
+        <v>1.0002438094285482</v>
+      </c>
+      <c r="J100" s="5">
+        <f t="shared" ref="J100:J104" si="47">G93/J93</f>
+        <v>1.2564392511622062</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="G101" s="5">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="H101" s="5">
+        <f t="shared" si="45"/>
+        <v>1.0088669950738915</v>
+      </c>
+      <c r="I101" s="5">
+        <f t="shared" si="46"/>
+        <v>1.0002438094285482</v>
+      </c>
+      <c r="J101" s="5">
+        <f t="shared" si="47"/>
+        <v>1.4553194198732964</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="G102" s="5">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="H102" s="5">
+        <f t="shared" si="45"/>
+        <v>1.2299563049336391</v>
+      </c>
+      <c r="I102" s="5">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="J102" s="5">
+        <f t="shared" si="47"/>
+        <v>1.7768676978211142</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="G103" s="5">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="H103" s="5">
+        <f t="shared" si="45"/>
+        <v>1.2302018535774548</v>
+      </c>
+      <c r="I103" s="5">
+        <f t="shared" si="46"/>
+        <v>1.0001996401358575</v>
+      </c>
+      <c r="J103" s="5">
+        <f t="shared" si="47"/>
+        <v>1.7772224319297081</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="G104" s="5">
+        <f t="shared" si="44"/>
+        <v>1</v>
+      </c>
+      <c r="H104" s="5">
+        <f t="shared" si="45"/>
+        <v>1.2302018535774548</v>
+      </c>
+      <c r="I104" s="5">
+        <f t="shared" si="46"/>
+        <v>1.0001996401358575</v>
+      </c>
+      <c r="J104" s="5">
+        <f t="shared" si="47"/>
+        <v>1.7772224319297081</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108">
+        <v>16</v>
+      </c>
+      <c r="C108" s="5">
+        <f>AVERAGE(G13,G48,G83)</f>
+        <v>1</v>
+      </c>
+      <c r="D108" s="5">
+        <f>AVERAGE(H13,H48,H83)</f>
+        <v>1.0240060305461489</v>
+      </c>
+      <c r="E108" s="5">
+        <f>AVERAGE(I13,I48,I83)</f>
+        <v>1.0622017764511569</v>
+      </c>
+      <c r="F108" s="5">
+        <f>AVERAGE(J13,J48,J83)</f>
+        <v>1.1926924559960146</v>
+      </c>
+      <c r="G108" s="5">
+        <f>AVERAGE(G29,G64,G99)</f>
+        <v>1</v>
+      </c>
+      <c r="H108" s="5">
+        <f>AVERAGE(H29,H64,H99)</f>
+        <v>1</v>
+      </c>
+      <c r="I108" s="5">
+        <f>AVERAGE(I29,I64,I99)</f>
+        <v>1.0107422015549845</v>
+      </c>
+      <c r="J108" s="5">
+        <f>AVERAGE(J29,J64,J99)</f>
+        <v>1.2232765777299919</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109">
+        <v>32</v>
+      </c>
+      <c r="C109" s="5">
+        <f t="shared" ref="C109:C113" si="48">AVERAGE(G14,G49,G84)</f>
+        <v>1</v>
+      </c>
+      <c r="D109" s="5">
+        <f t="shared" ref="D109:D113" si="49">AVERAGE(H14,H49,H84)</f>
+        <v>1.0317378779667303</v>
+      </c>
+      <c r="E109" s="5">
+        <f t="shared" ref="E109:E113" si="50">AVERAGE(I14,I49,I84)</f>
+        <v>1.0128464152317593</v>
+      </c>
+      <c r="F109" s="5">
+        <f t="shared" ref="F109:F113" si="51">AVERAGE(J14,J49,J84)</f>
+        <v>1.1155647320986419</v>
+      </c>
+      <c r="G109" s="5">
+        <f t="shared" ref="G109:J113" si="52">AVERAGE(G30,G65,G100)</f>
+        <v>1</v>
+      </c>
+      <c r="H109" s="5">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="I109" s="5">
+        <f t="shared" si="52"/>
+        <v>1.0110071981261315</v>
+      </c>
+      <c r="J109" s="5">
+        <f t="shared" si="52"/>
+        <v>1.2369586024124011</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110">
+        <v>64</v>
+      </c>
+      <c r="C110" s="5">
+        <f t="shared" si="48"/>
+        <v>1</v>
+      </c>
+      <c r="D110" s="5">
+        <f t="shared" si="49"/>
+        <v>1.0323415039999784</v>
+      </c>
+      <c r="E110" s="5">
+        <f t="shared" si="50"/>
+        <v>1.0316498151574207</v>
+      </c>
+      <c r="F110" s="5">
+        <f t="shared" si="51"/>
+        <v>1.0450146814441998</v>
+      </c>
+      <c r="G110" s="5">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="H110" s="5">
+        <f t="shared" si="52"/>
+        <v>1.0029556650246305</v>
+      </c>
+      <c r="I110" s="5">
+        <f t="shared" si="52"/>
+        <v>1.0070179939339718</v>
+      </c>
+      <c r="J110" s="5">
+        <f t="shared" si="52"/>
+        <v>1.6773334521005197</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111">
+        <v>128</v>
+      </c>
+      <c r="C111" s="5">
+        <f t="shared" si="48"/>
+        <v>1</v>
+      </c>
+      <c r="D111" s="5">
+        <f t="shared" si="49"/>
+        <v>1.0009404346259043</v>
+      </c>
+      <c r="E111" s="5">
+        <f t="shared" si="50"/>
+        <v>1.0004036305298485</v>
+      </c>
+      <c r="F111" s="5">
+        <f t="shared" si="51"/>
+        <v>1.0009404346259043</v>
+      </c>
+      <c r="G111" s="5">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="H111" s="5">
+        <f t="shared" si="52"/>
+        <v>1.4282646543871624</v>
+      </c>
+      <c r="I111" s="5">
+        <f t="shared" si="52"/>
+        <v>1.0653294731057226</v>
+      </c>
+      <c r="J111" s="5">
+        <f t="shared" si="52"/>
+        <v>2.8254011484049912</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112">
+        <v>256</v>
+      </c>
+      <c r="C112" s="5">
+        <f t="shared" si="48"/>
+        <v>1</v>
+      </c>
+      <c r="D112" s="5">
+        <f t="shared" si="49"/>
+        <v>1.0005190677595623</v>
+      </c>
+      <c r="E112" s="5">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="F112" s="5">
+        <f t="shared" si="51"/>
+        <v>1.0005190677595623</v>
+      </c>
+      <c r="G112" s="5">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="H112" s="5">
+        <f t="shared" si="52"/>
+        <v>1.4379955545680125</v>
+      </c>
+      <c r="I112" s="5">
+        <f t="shared" si="52"/>
+        <v>1.0720816727234901</v>
+      </c>
+      <c r="J112" s="5">
+        <f t="shared" si="52"/>
+        <v>2.8402445312321931</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113">
+        <v>512</v>
+      </c>
+      <c r="C113" s="5">
+        <f t="shared" si="48"/>
+        <v>1</v>
+      </c>
+      <c r="D113" s="5">
+        <f t="shared" si="49"/>
+        <v>1.0005190677595623</v>
+      </c>
+      <c r="E113" s="5">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="F113" s="5">
+        <f t="shared" si="51"/>
+        <v>1.0005190677595623</v>
+      </c>
+      <c r="G113" s="5">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="H113" s="5">
+        <f t="shared" si="52"/>
+        <v>1.4379955545680125</v>
+      </c>
+      <c r="I113" s="5">
+        <f t="shared" si="52"/>
+        <v>1.0720816727234901</v>
+      </c>
+      <c r="J113" s="5">
+        <f t="shared" si="52"/>
+        <v>2.8402445312321931</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G82:J82"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4928,8 +6082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="O79" sqref="O79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>